<commit_message>
2018-01-02 : 회로 및 PCB 수정 Plasma CON pin-map 및 Pulse에 저항 추가 Charging IC PCB Library 수정
</commit_message>
<xml_diff>
--- a/V2.0/Plasma Generator_Part List_V2.0_20171222.xlsx
+++ b/V2.0/Plasma Generator_Part List_V2.0_20171222.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\My_Work\20171116_FemtoScience\1_Schematic\V2.0\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\My_Work\20171116_FemtoScience\4_Firmware\Plasma_Gen_Git\V2.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1">'Main Board'!$B$5:$M$5</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="152511" calcMode="manual"/>
 </workbook>
 </file>
 
@@ -853,10 +853,6 @@
     <phoneticPr fontId="19" type="noConversion"/>
   </si>
   <si>
-    <t>R26,R27,R30</t>
-    <phoneticPr fontId="19" type="noConversion"/>
-  </si>
-  <si>
     <t>Total</t>
     <phoneticPr fontId="19" type="noConversion"/>
   </si>
@@ -952,6 +948,10 @@
   </si>
   <si>
     <t>R10</t>
+    <phoneticPr fontId="19" type="noConversion"/>
+  </si>
+  <si>
+    <t>R26,R27,R30,R35,R36</t>
     <phoneticPr fontId="19" type="noConversion"/>
   </si>
 </sst>
@@ -2226,9 +2226,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2254,6 +2251,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2600,16 +2600,16 @@
     <row r="2" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="3" spans="2:5" s="17" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="94" t="s">
+        <v>249</v>
+      </c>
+      <c r="C3" s="91" t="s">
         <v>250</v>
       </c>
-      <c r="C3" s="91" t="s">
+      <c r="D3" s="91" t="s">
         <v>251</v>
       </c>
-      <c r="D3" s="91" t="s">
-        <v>252</v>
-      </c>
       <c r="E3" s="95" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.3">
@@ -2617,13 +2617,13 @@
         <v>43082</v>
       </c>
       <c r="C4" s="8" t="s">
+        <v>252</v>
+      </c>
+      <c r="D4" s="8" t="s">
         <v>253</v>
       </c>
-      <c r="D4" s="8" t="s">
-        <v>254</v>
-      </c>
       <c r="E4" s="97" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.3">
@@ -2809,7 +2809,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F25" sqref="F25"/>
+      <selection pane="bottomLeft" activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2857,7 +2857,7 @@
         <v>136</v>
       </c>
       <c r="H3" s="69" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="U3" s="16" t="s">
         <v>191</v>
@@ -2901,10 +2901,10 @@
         <v>6</v>
       </c>
       <c r="H5" s="27" t="s">
+        <v>244</v>
+      </c>
+      <c r="I5" s="27" t="s">
         <v>245</v>
-      </c>
-      <c r="I5" s="27" t="s">
-        <v>246</v>
       </c>
       <c r="J5" s="27" t="s">
         <v>7</v>
@@ -3120,7 +3120,7 @@
       </c>
       <c r="I8" s="65"/>
       <c r="J8" s="71" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="K8" s="68" t="s">
         <v>138</v>
@@ -3389,16 +3389,16 @@
       <c r="F12" s="64" t="s">
         <v>54</v>
       </c>
-      <c r="G12" s="65">
-        <v>3</v>
+      <c r="G12" s="70">
+        <v>5</v>
       </c>
       <c r="H12" s="65">
         <f t="shared" si="3"/>
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="I12" s="65"/>
-      <c r="J12" s="64" t="s">
-        <v>244</v>
+      <c r="J12" s="32" t="s">
+        <v>268</v>
       </c>
       <c r="K12" s="68" t="s">
         <v>138</v>
@@ -3414,7 +3414,7 @@
       </c>
       <c r="O12" s="60">
         <f t="shared" si="0"/>
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="P12" s="57">
         <v>100</v>
@@ -3434,7 +3434,7 @@
       </c>
       <c r="U12" s="74">
         <f t="shared" si="2"/>
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="V12" s="36" t="s">
         <v>194</v>
@@ -3524,10 +3524,10 @@
         <v>36</v>
       </c>
       <c r="E14" s="32" t="s">
+        <v>256</v>
+      </c>
+      <c r="F14" s="32" t="s">
         <v>257</v>
-      </c>
-      <c r="F14" s="32" t="s">
-        <v>258</v>
       </c>
       <c r="G14" s="70">
         <v>4</v>
@@ -3538,7 +3538,7 @@
       </c>
       <c r="I14" s="65"/>
       <c r="J14" s="32" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="K14" s="26" t="s">
         <v>138</v>
@@ -3608,7 +3608,7 @@
       </c>
       <c r="I15" s="65"/>
       <c r="J15" s="32" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="K15" s="26" t="s">
         <v>138</v>
@@ -3798,18 +3798,18 @@
         <v>12</v>
       </c>
       <c r="C18" s="65" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D18" s="65" t="s">
         <v>36</v>
       </c>
       <c r="E18" s="64" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="F18" s="64" t="s">
-        <v>264</v>
-      </c>
-      <c r="G18" s="102">
+        <v>263</v>
+      </c>
+      <c r="G18" s="101">
         <v>16</v>
       </c>
       <c r="H18" s="65">
@@ -3818,7 +3818,7 @@
       </c>
       <c r="I18" s="65"/>
       <c r="J18" s="72" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="K18" s="68" t="s">
         <v>138</v>
@@ -3938,16 +3938,16 @@
         <v>14</v>
       </c>
       <c r="C20" s="70" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="D20" s="70" t="s">
         <v>36</v>
       </c>
       <c r="E20" s="32" t="s">
+        <v>261</v>
+      </c>
+      <c r="F20" s="32" t="s">
         <v>262</v>
-      </c>
-      <c r="F20" s="32" t="s">
-        <v>263</v>
       </c>
       <c r="G20" s="65">
         <v>1</v>
@@ -3958,7 +3958,7 @@
       </c>
       <c r="I20" s="65"/>
       <c r="J20" s="32" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="K20" s="26" t="s">
         <v>138</v>
@@ -4693,7 +4693,7 @@
         <v>101</v>
       </c>
       <c r="F30" s="64" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="G30" s="65">
         <v>1</v>
@@ -5151,7 +5151,7 @@
         <v>128</v>
       </c>
       <c r="F36" s="64" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="G36" s="65">
         <v>1</v>
@@ -5458,7 +5458,7 @@
       <c r="E40" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="F40" s="103" t="s">
+      <c r="F40" s="102" t="s">
         <v>143</v>
       </c>
       <c r="G40" s="65">
@@ -5517,10 +5517,10 @@
       <c r="E41" s="43" t="s">
         <v>143</v>
       </c>
-      <c r="F41" s="104" t="s">
+      <c r="F41" s="103" t="s">
         <v>227</v>
       </c>
-      <c r="G41" s="105">
+      <c r="G41" s="104">
         <v>4</v>
       </c>
       <c r="H41" s="65">
@@ -5574,7 +5574,7 @@
       <c r="E42" s="8" t="s">
         <v>208</v>
       </c>
-      <c r="F42" s="106" t="s">
+      <c r="F42" s="105" t="s">
         <v>212</v>
       </c>
       <c r="G42" s="46">
@@ -5587,7 +5587,7 @@
       <c r="I42" s="46">
         <v>20</v>
       </c>
-      <c r="J42" s="106"/>
+      <c r="J42" s="105"/>
       <c r="K42" s="8"/>
       <c r="L42" s="7"/>
       <c r="M42" s="7"/>
@@ -5635,10 +5635,10 @@
       <c r="E43" s="22" t="s">
         <v>210</v>
       </c>
-      <c r="F43" s="107" t="s">
+      <c r="F43" s="106" t="s">
         <v>214</v>
       </c>
-      <c r="G43" s="108">
+      <c r="G43" s="107">
         <f>3*4*2</f>
         <v>24</v>
       </c>
@@ -5646,10 +5646,10 @@
         <f t="shared" si="3"/>
         <v>72</v>
       </c>
-      <c r="I43" s="108">
+      <c r="I43" s="107">
         <v>100</v>
       </c>
-      <c r="J43" s="107"/>
+      <c r="J43" s="106"/>
       <c r="K43" s="22"/>
       <c r="L43" s="23"/>
       <c r="M43" s="23"/>
@@ -5688,14 +5688,14 @@
     </row>
     <row r="44" spans="1:25" x14ac:dyDescent="0.3">
       <c r="F44" s="63"/>
-      <c r="G44" s="102"/>
-      <c r="H44" s="102"/>
-      <c r="I44" s="102"/>
+      <c r="G44" s="101"/>
+      <c r="H44" s="101"/>
+      <c r="I44" s="101"/>
       <c r="J44" s="63"/>
       <c r="N44" s="2"/>
       <c r="O44" s="3">
         <f>SUM(O6:O41)</f>
-        <v>21630</v>
+        <v>21650</v>
       </c>
       <c r="Q44" s="3">
         <f>SUM(Q6:Q41)</f>
@@ -5715,11 +5715,11 @@
       <c r="A45" s="16"/>
       <c r="C45" s="17"/>
       <c r="D45" s="17"/>
-      <c r="F45" s="109"/>
-      <c r="G45" s="110"/>
-      <c r="H45" s="110"/>
-      <c r="I45" s="110"/>
-      <c r="J45" s="109"/>
+      <c r="F45" s="108"/>
+      <c r="G45" s="109"/>
+      <c r="H45" s="109"/>
+      <c r="I45" s="109"/>
+      <c r="J45" s="108"/>
       <c r="L45" s="17"/>
       <c r="M45" s="17"/>
       <c r="Q45" s="16"/>
@@ -5824,10 +5824,10 @@
       </c>
     </row>
     <row r="6" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B6" s="101">
+      <c r="B6" s="110">
         <v>1</v>
       </c>
-      <c r="C6" s="101" t="s">
+      <c r="C6" s="110" t="s">
         <v>161</v>
       </c>
       <c r="D6" s="18" t="s">
@@ -5854,8 +5854,8 @@
       </c>
     </row>
     <row r="7" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B7" s="101"/>
-      <c r="C7" s="101"/>
+      <c r="B7" s="110"/>
+      <c r="C7" s="110"/>
       <c r="D7" s="18" t="s">
         <v>165</v>
       </c>
@@ -5873,8 +5873,8 @@
       </c>
     </row>
     <row r="8" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B8" s="101"/>
-      <c r="C8" s="101"/>
+      <c r="B8" s="110"/>
+      <c r="C8" s="110"/>
       <c r="D8" s="18" t="s">
         <v>166</v>
       </c>
@@ -5883,10 +5883,10 @@
       </c>
     </row>
     <row r="9" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B9" s="101">
+      <c r="B9" s="110">
         <v>2</v>
       </c>
-      <c r="C9" s="101" t="s">
+      <c r="C9" s="110" t="s">
         <v>162</v>
       </c>
       <c r="D9" s="18" t="s">
@@ -5900,8 +5900,8 @@
       </c>
     </row>
     <row r="10" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B10" s="101"/>
-      <c r="C10" s="101"/>
+      <c r="B10" s="110"/>
+      <c r="C10" s="110"/>
       <c r="D10" s="18" t="s">
         <v>165</v>
       </c>
@@ -5910,10 +5910,10 @@
       </c>
     </row>
     <row r="11" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B11" s="101">
+      <c r="B11" s="110">
         <v>3</v>
       </c>
-      <c r="C11" s="101" t="s">
+      <c r="C11" s="110" t="s">
         <v>163</v>
       </c>
       <c r="D11" s="18" t="s">
@@ -5927,8 +5927,8 @@
       </c>
     </row>
     <row r="12" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B12" s="101"/>
-      <c r="C12" s="101"/>
+      <c r="B12" s="110"/>
+      <c r="C12" s="110"/>
       <c r="D12" s="18" t="s">
         <v>165</v>
       </c>
@@ -5940,8 +5940,8 @@
       </c>
     </row>
     <row r="13" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B13" s="101"/>
-      <c r="C13" s="101"/>
+      <c r="B13" s="110"/>
+      <c r="C13" s="110"/>
       <c r="D13" s="18" t="s">
         <v>166</v>
       </c>

</xml_diff>